<commit_message>
- On grid, checkbox filter need to be linked with approved/not-approved - FicheMessage - Edit - A/R replace it with "Approuvée" and "Approved" - Remove the isActive and link it with isApproved it - FicheCadeassage/editfiche - add button "Archiver" and "Archive" - Remove Simdut 2015 and Formation - Make header fixed - Analyse de Risque  [row 1, 2, and 3] - Add page number when printing [all sheets in Analyse de Risque] if possible
</commit_message>
<xml_diff>
--- a/Previgesst/Templates/AnalyseRisques.xlsx
+++ b/Previgesst/Templates/AnalyseRisques.xlsx
@@ -1670,7 +1670,8 @@
   <dimension ref="A1:X485"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -12090,8 +12091,11 @@
       <formula>"Oui"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.19685039370078741" footer="0.19685039370078741"/>
-  <pageSetup paperSize="5" scale="55" fitToHeight="100" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.196850393700787" right="0.196850393700787" top="0.196850393700787" bottom="0.196850393700787" header="0.196850393700787" footer="0.196850393700787"/>
+  <pageSetup paperSize="5" scale="58" fitToHeight="100" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -12104,7 +12108,8 @@
   <dimension ref="A1:H646"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -16686,8 +16691,11 @@
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="A1:D2"/>
   </mergeCells>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="5" scale="68" fitToHeight="100" orientation="landscape"/>
+  <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="5" scale="65" fitToHeight="100" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>